<commit_message>
Create hydrogen supply dataset for each region
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-heating.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-heating.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172171E5-51CD-A64A-AA80-550E271CE998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8828EB46-C4A9-704A-AE41-DDEE5691C2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36580" yWindow="1660" windowWidth="26840" windowHeight="15940" xr2:uid="{CF516D2F-FFD4-214F-BF62-5C2F0868DC96}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23000" xr2:uid="{CF516D2F-FFD4-214F-BF62-5C2F0868DC96}"/>
   </bookViews>
   <sheets>
     <sheet name="hydrogen boiler" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'hydrogen boiler'!$A$1:$W$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'hydrogen boiler'!$A$1:$W$113</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="121">
   <si>
     <t>Activity</t>
   </si>
@@ -390,6 +390,18 @@
   </si>
   <si>
     <t>cubic meter</t>
+  </si>
+  <si>
+    <t>hydrogen supply, distributed by pipeline</t>
+  </si>
+  <si>
+    <t>market for hydrogen, gaseous</t>
+  </si>
+  <si>
+    <t>hydrogen, gaseous</t>
+  </si>
+  <si>
+    <t>This dataset represents the supply of 1 kilogram of hydrogen. The hydrogen is distributed by pipeline over 250 km to the regional storage (Geological cavity) and transported another 250 km to the consumer.  The hydrogen represents the market average for the region. Transmission loss [% output]: 0.0007125%. Regional storage loss [% output]: 0.69.  Arrives at 30 bar of pressure. For more information, refer to: Sacchi, R. and Bauer, C. LCA of Power-to-X processes and applications in the residential sector. Paul Scherrer Institut, 2023.</t>
   </si>
 </sst>
 </file>
@@ -798,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2FA153-E6EA-3E4B-BE1A-EC0443996927}">
-  <dimension ref="A1:W93"/>
+  <dimension ref="A1:W113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -824,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
@@ -832,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -848,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
@@ -959,7 +971,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -968,7 +980,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
         <v>30</v>
@@ -979,7 +991,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -988,13 +1000,13 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
         <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="H13" t="s">
         <v>11</v>
@@ -1035,7 +1047,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="B14">
         <v>6.9143483761158198E-3</v>
@@ -1044,13 +1056,13 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
         <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="H14" t="s">
         <v>11</v>
@@ -1201,7 +1213,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1257,7 +1269,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1313,7 +1325,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>113</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>52</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F19" t="s">
         <v>32</v>
@@ -1369,7 +1381,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -1380,7 +1392,7 @@
         <v>52</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
         <v>32</v>
@@ -1425,7 +1437,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>52</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
         <v>32</v>
@@ -1481,7 +1493,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1534,836 +1546,888 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J31" s="2" t="s">
+      <c r="I31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="L31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="M31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="N31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O31" s="2" t="s">
+      <c r="O31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P31" s="2" t="s">
+      <c r="P31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="Q31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="R31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S31" s="2" t="s">
+      <c r="S31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="T31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U31" s="2"/>
-    </row>
-    <row r="32" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>95</v>
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
       </c>
       <c r="E32" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" t="s">
         <v>30</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="7">
-        <v>3.984190731178683E-7</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>1.5</v>
+      </c>
+      <c r="M33">
+        <v>1.2</v>
+      </c>
+      <c r="N33">
+        <v>1.5</v>
+      </c>
+      <c r="O33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P33">
+        <v>2</v>
+      </c>
+      <c r="Q33">
+        <v>1.2</v>
+      </c>
+      <c r="R33">
+        <v>1.05</v>
+      </c>
+      <c r="S33">
+        <v>0.47095746419981693</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>6.9143483761158198E-3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" t="s">
+        <v>35</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>-4.9741565516945512</v>
+      </c>
+      <c r="L34">
+        <v>1.5</v>
+      </c>
+      <c r="M34">
+        <v>1.2</v>
+      </c>
+      <c r="N34">
+        <v>1.5</v>
+      </c>
+      <c r="O34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P34">
+        <v>2</v>
+      </c>
+      <c r="Q34">
+        <v>1.2</v>
+      </c>
+      <c r="R34">
+        <v>1.05</v>
+      </c>
+      <c r="S34">
+        <v>0.47095746419981693</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>1.1442208504274044E-6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" t="s">
+        <v>38</v>
+      </c>
+      <c r="H35" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" t="s">
+        <v>40</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35">
+        <v>-13.680786632565722</v>
+      </c>
+      <c r="L35">
+        <v>1.5</v>
+      </c>
+      <c r="M35">
+        <v>1.2</v>
+      </c>
+      <c r="N35">
+        <v>1.5</v>
+      </c>
+      <c r="O35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P35">
+        <v>2</v>
+      </c>
+      <c r="Q35">
+        <v>1.2</v>
+      </c>
+      <c r="R35">
+        <v>3</v>
+      </c>
+      <c r="S35">
+        <v>0.72314801614797197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>2.0170559863303602E-9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" t="s">
+        <v>39</v>
+      </c>
+      <c r="I36" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+      <c r="K36">
+        <v>-20.021626821130827</v>
+      </c>
+      <c r="L36">
+        <v>1.5</v>
+      </c>
+      <c r="M36">
+        <v>1.2</v>
+      </c>
+      <c r="N36">
+        <v>1.5</v>
+      </c>
+      <c r="O36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P36">
+        <v>2</v>
+      </c>
+      <c r="Q36">
+        <v>1.2</v>
+      </c>
+      <c r="R36">
+        <v>3</v>
+      </c>
+      <c r="S36">
+        <v>0.72314801614797197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>3.2270310019264991E-11</v>
+      </c>
+      <c r="C37" t="s">
         <v>9</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J33" s="4">
-        <v>2</v>
-      </c>
-      <c r="K33" s="4">
-        <v>-14.735761438090067</v>
-      </c>
-      <c r="L33" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M33" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N33" s="4">
-        <v>1</v>
-      </c>
-      <c r="O33" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P33" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q33" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R33" s="4">
-        <v>3</v>
-      </c>
-      <c r="S33" s="4">
-        <v>0.57209088006881903</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="7">
-        <v>7.9683814623573661E-7</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J34" s="4">
-        <v>2</v>
-      </c>
-      <c r="K34" s="4">
-        <v>-14.042614257530122</v>
-      </c>
-      <c r="L34" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M34" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N34" s="4">
-        <v>1</v>
-      </c>
-      <c r="O34" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P34" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q34" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R34" s="4">
-        <v>3</v>
-      </c>
-      <c r="S34" s="4">
-        <v>0.57209088006881903</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B35" s="7">
-        <v>7.3399999999999995E-4</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J35" s="4">
-        <v>2</v>
-      </c>
-      <c r="K35" s="4">
-        <v>-7.2170015293497585</v>
-      </c>
-      <c r="L35" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M35" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N35" s="4">
-        <v>1</v>
-      </c>
-      <c r="O35" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P35" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q35" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R35" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S35" s="4">
-        <v>0.16169679924070957</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="9">
-        <v>7.5075075075075066E-3</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" t="s">
-        <v>45</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J36" s="4">
-        <v>2</v>
-      </c>
-      <c r="K36" s="4">
-        <v>-4.8918517581062888</v>
-      </c>
-      <c r="L36" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M36" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N36" s="4">
-        <v>1</v>
-      </c>
-      <c r="O36" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P36" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q36" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R36" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S36" s="4">
-        <v>0.16169679924070957</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="9">
-        <v>3.7537537537536729E-5</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="E37" t="s">
         <v>45</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J37" s="4">
-        <v>2</v>
-      </c>
-      <c r="K37" s="4">
-        <v>-10.190169124654346</v>
-      </c>
-      <c r="L37" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M37" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N37" s="4">
-        <v>1</v>
-      </c>
-      <c r="O37" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P37" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q37" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R37" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S37" s="4">
-        <v>0.16169679924070957</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="5">
-        <f>0.0675675675675676/1000</f>
-        <v>6.7567567567567596E-5</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="G37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" t="s">
+        <v>39</v>
+      </c>
+      <c r="I37" t="s">
+        <v>47</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
+        <v>-24.156873502868216</v>
+      </c>
+      <c r="L37">
+        <v>1.5</v>
+      </c>
+      <c r="M37">
+        <v>1.2</v>
+      </c>
+      <c r="N37">
+        <v>1.5</v>
+      </c>
+      <c r="O37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P37">
+        <v>2</v>
+      </c>
+      <c r="Q37">
+        <v>1.2</v>
+      </c>
+      <c r="R37">
+        <v>3</v>
+      </c>
+      <c r="S37">
+        <v>0.72314801614797197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38">
+        <v>0.30207430451283473</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" t="s">
+        <v>39</v>
+      </c>
+      <c r="I38" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>-1.1970822504372693</v>
+      </c>
+      <c r="L38">
+        <v>1.5</v>
+      </c>
+      <c r="M38">
+        <v>1.2</v>
+      </c>
+      <c r="N38">
+        <v>1.5</v>
+      </c>
+      <c r="O38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P38">
+        <v>2</v>
+      </c>
+      <c r="Q38">
+        <v>1.2</v>
+      </c>
+      <c r="R38">
+        <v>3</v>
+      </c>
+      <c r="S38">
+        <v>0.72314801614797197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39">
+        <v>1.0291066405763645</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <v>2.8691086638977469E-2</v>
+      </c>
+      <c r="L39">
+        <v>1.5</v>
+      </c>
+      <c r="M39">
+        <v>1.2</v>
+      </c>
+      <c r="N39">
+        <v>1.5</v>
+      </c>
+      <c r="O39">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P39">
+        <v>2</v>
+      </c>
+      <c r="Q39">
+        <v>1.2</v>
+      </c>
+      <c r="R39">
+        <v>1.05</v>
+      </c>
+      <c r="S39">
+        <v>0.47095746419981693</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40">
+        <v>0.64442518296071416</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" t="s">
+        <v>55</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
+        <v>-0.43939654873975276</v>
+      </c>
+      <c r="L40">
+        <v>1.5</v>
+      </c>
+      <c r="M40">
+        <v>1.2</v>
+      </c>
+      <c r="N40">
+        <v>1.5</v>
+      </c>
+      <c r="O40">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P40">
+        <v>2</v>
+      </c>
+      <c r="Q40">
+        <v>1.2</v>
+      </c>
+      <c r="R40">
+        <v>1.05</v>
+      </c>
+      <c r="S40">
+        <v>0.47095746419981693</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41">
+        <v>0.14302201400538245</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="s">
+        <v>53</v>
+      </c>
+      <c r="H41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" t="s">
+        <v>56</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>-1.9447567164768222</v>
+      </c>
+      <c r="L41">
+        <v>1.5</v>
+      </c>
+      <c r="M41">
+        <v>1.2</v>
+      </c>
+      <c r="N41">
+        <v>1.5</v>
+      </c>
+      <c r="O41">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P41">
+        <v>2</v>
+      </c>
+      <c r="Q41">
+        <v>1.2</v>
+      </c>
+      <c r="R41">
+        <v>1.05</v>
+      </c>
+      <c r="S41">
+        <v>0.47095746419981693</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <v>6.9143483761158198E-3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F42" t="s">
         <v>59</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H42" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J38" s="4">
-        <v>2</v>
-      </c>
-      <c r="K38" s="4">
-        <v>-2.6946271807700697</v>
-      </c>
-      <c r="L38" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M38" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N38" s="4">
-        <v>1</v>
-      </c>
-      <c r="O38" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P38" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q38" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R38" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S38" s="4">
-        <v>0.16169679924070957</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="5">
-        <v>6.9444444444444448E-6</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J39" s="4">
-        <v>2</v>
-      </c>
-      <c r="K39" s="4">
-        <v>-11.877568578558138</v>
-      </c>
-      <c r="L39" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M39" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N39" s="4">
-        <v>1</v>
-      </c>
-      <c r="O39" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P39" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q39" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R39" s="4">
+      <c r="I42" t="s">
+        <v>61</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <v>-4.9741565516945512</v>
+      </c>
+      <c r="L42">
         <v>1.5</v>
       </c>
-      <c r="S39" s="4">
-        <v>0.25816898211842121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="9">
-        <v>3.7537537537536729E-5</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="M40" s="8"/>
-    </row>
-    <row r="41" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="5"/>
-    </row>
-    <row r="42" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="M42">
+        <v>1.2</v>
+      </c>
+      <c r="N42">
+        <v>1.5</v>
+      </c>
+      <c r="O42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P42">
+        <v>2</v>
+      </c>
+      <c r="Q42">
+        <v>1.2</v>
+      </c>
+      <c r="R42">
+        <v>1.05</v>
+      </c>
+      <c r="S42">
+        <v>0.47095746419981693</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>5</v>
+      <c r="B44" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+    <row r="50" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="5"/>
-    </row>
-    <row r="49" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="B50" s="5"/>
+    </row>
+    <row r="51" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J49" s="2" t="s">
+      <c r="I51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="K51" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L49" s="2" t="s">
+      <c r="L51" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="M51" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N49" s="2" t="s">
+      <c r="N51" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O49" s="2" t="s">
+      <c r="O51" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P49" s="2" t="s">
+      <c r="P51" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q49" s="2" t="s">
+      <c r="Q51" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R49" s="2" t="s">
+      <c r="R51" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S49" s="2" t="s">
+      <c r="S51" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T49" s="2" t="s">
+      <c r="T51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U49" s="2"/>
-    </row>
-    <row r="50" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B50" s="5">
-        <v>1</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="7">
-        <v>6.509296454909041E-10</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J51" s="4">
-        <v>2</v>
-      </c>
-      <c r="K51" s="4">
-        <v>-21.152619551002662</v>
-      </c>
-      <c r="L51" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M51" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N51" s="4">
-        <v>1</v>
-      </c>
-      <c r="O51" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P51" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q51" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R51" s="4">
-        <v>3</v>
-      </c>
-      <c r="S51" s="4">
-        <v>0.57209088006881903</v>
-      </c>
+      <c r="U51" s="2"/>
     </row>
     <row r="52" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="7">
-        <v>6.509296454909041E-10</v>
+        <v>92</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" t="s">
         <v>45</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J52" s="4">
-        <v>2</v>
-      </c>
-      <c r="K52" s="4">
-        <v>-21.152619551002662</v>
-      </c>
-      <c r="L52" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M52" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N52" s="4">
-        <v>1</v>
-      </c>
-      <c r="O52" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="P52" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q52" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R52" s="4">
-        <v>3</v>
-      </c>
-      <c r="S52" s="4">
-        <v>0.57209088006881903</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="B53" s="7">
-        <v>6.509296454909041E-10</v>
+        <v>3.984190731178683E-7</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>39</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J53" s="4">
         <v>2</v>
       </c>
       <c r="K53" s="4">
-        <v>-21.152619551002662</v>
+        <v>-14.735761438090067</v>
       </c>
       <c r="L53" s="4">
         <v>1.05</v>
@@ -2392,31 +2456,34 @@
     </row>
     <row r="54" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B54" s="7">
-        <v>9.4583599412497203E-9</v>
+        <v>7.9683814623573661E-7</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>79</v>
+        <v>39</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="J54" s="4">
         <v>2</v>
       </c>
       <c r="K54" s="4">
-        <v>-18.476366836645134</v>
+        <v>-14.042614257530122</v>
       </c>
       <c r="L54" s="4">
         <v>1.05</v>
@@ -2437,39 +2504,42 @@
         <v>1.2</v>
       </c>
       <c r="R54" s="4">
-        <v>1.05</v>
+        <v>3</v>
       </c>
       <c r="S54" s="4">
-        <v>0.16169679924070957</v>
+        <v>0.57209088006881903</v>
       </c>
     </row>
     <row r="55" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="B55" s="7">
-        <v>-9.4583599412497203E-9</v>
+        <v>7.3399999999999995E-4</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>114</v>
+        <v>52</v>
+      </c>
+      <c r="E55" t="s">
+        <v>45</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>79</v>
+        <v>12</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="J55" s="4">
-        <v>1</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>51</v>
+        <v>2</v>
+      </c>
+      <c r="K55" s="4">
+        <v>-7.2170015293497585</v>
       </c>
       <c r="L55" s="4">
         <v>1.05</v>
@@ -2490,13 +2560,10 @@
         <v>1.2</v>
       </c>
       <c r="R55" s="4">
-        <v>3</v>
+        <v>1.05</v>
       </c>
       <c r="S55" s="4">
-        <v>0.57209088006881903</v>
-      </c>
-      <c r="T55" s="4" t="b">
-        <v>1</v>
+        <v>0.16169679924070957</v>
       </c>
     </row>
     <row r="56" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2504,12 +2571,12 @@
         <v>1</v>
       </c>
       <c r="B56" s="9">
-        <v>1.6629947742052215E-3</v>
+        <v>7.5075075075075066E-3</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" t="s">
         <v>45</v>
       </c>
       <c r="F56" s="4" t="s">
@@ -2528,7 +2595,7 @@
         <v>2</v>
       </c>
       <c r="K56" s="4">
-        <v>-6.399135221166409</v>
+        <v>-4.8918517581062888</v>
       </c>
       <c r="L56" s="4">
         <v>1.05</v>
@@ -2560,12 +2627,12 @@
         <v>1</v>
       </c>
       <c r="B57" s="9">
-        <v>8.31497387102593E-6</v>
+        <v>3.7537537537536729E-5</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" t="s">
         <v>45</v>
       </c>
       <c r="F57" s="4" t="s">
@@ -2584,7 +2651,7 @@
         <v>2</v>
       </c>
       <c r="K57" s="4">
-        <v>-11.697452587714467</v>
+        <v>-10.190169124654346</v>
       </c>
       <c r="L57" s="4">
         <v>1.05</v>
@@ -2616,8 +2683,8 @@
         <v>87</v>
       </c>
       <c r="B58" s="5">
-        <f>0.014966952967847/1000</f>
-        <v>1.4966952967847001E-5</v>
+        <f>0.0675675675675676/1000</f>
+        <v>6.7567567567567596E-5</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>116</v>
@@ -2638,7 +2705,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="4">
-        <v>-4.2019106438301899</v>
+        <v>-2.6946271807700697</v>
       </c>
       <c r="L58" s="4">
         <v>1.05</v>
@@ -2723,7 +2790,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="9">
-        <v>8.31497387102593E-6</v>
+        <v>3.7537537537536729E-5</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>10</v>
@@ -2750,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2758,7 +2825,7 @@
         <v>2</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2864,7 +2931,7 @@
     </row>
     <row r="70" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B70" s="5">
         <v>1</v>
@@ -2884,37 +2951,37 @@
     </row>
     <row r="71" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B71" s="7">
-        <v>6.2590774062544461E-7</v>
+        <v>6.509296454909041E-10</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>39</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J71" s="4">
         <v>2</v>
       </c>
       <c r="K71" s="4">
-        <v>-14.284062855900274</v>
+        <v>-21.152619551002662</v>
       </c>
       <c r="L71" s="4">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="M71" s="8">
         <v>1.2</v>
@@ -2935,39 +3002,39 @@
         <v>3</v>
       </c>
       <c r="S71" s="4">
-        <v>0.57157051623399524</v>
+        <v>0.57209088006881903</v>
       </c>
     </row>
     <row r="72" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B72" s="9">
-        <v>2.0556127902646181E-3</v>
+        <v>98</v>
+      </c>
+      <c r="B72" s="7">
+        <v>6.509296454909041E-10</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="J72" s="4">
         <v>2</v>
       </c>
       <c r="K72" s="4">
-        <v>-6.1871812807091953</v>
+        <v>-21.152619551002662</v>
       </c>
       <c r="L72" s="4">
         <v>1.05</v>
@@ -2988,42 +3055,42 @@
         <v>1.2</v>
       </c>
       <c r="R72" s="4">
-        <v>1.05</v>
+        <v>3</v>
       </c>
       <c r="S72" s="4">
-        <v>0.16169679924070957</v>
+        <v>0.57209088006881903</v>
       </c>
     </row>
     <row r="73" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="9">
-        <v>1.1511431625481964E-5</v>
+        <v>100</v>
+      </c>
+      <c r="B73" s="7">
+        <v>6.509296454909041E-10</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="J73" s="4">
         <v>2</v>
       </c>
       <c r="K73" s="4">
-        <v>-11.37216996195022</v>
+        <v>-21.152619551002662</v>
       </c>
       <c r="L73" s="4">
         <v>1.05</v>
@@ -3044,590 +3111,1250 @@
         <v>1.2</v>
       </c>
       <c r="R73" s="4">
-        <v>1.05</v>
+        <v>3</v>
       </c>
       <c r="S73" s="4">
-        <v>0.16169679924070957</v>
+        <v>0.57209088006881903</v>
       </c>
     </row>
     <row r="74" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" s="7">
+        <v>9.4583599412497203E-9</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J74" s="4">
+        <v>2</v>
+      </c>
+      <c r="K74" s="4">
+        <v>-18.476366836645134</v>
+      </c>
+      <c r="L74" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N74" s="4">
+        <v>1</v>
+      </c>
+      <c r="O74" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P74" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q74" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R74" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S74" s="4">
+        <v>0.16169679924070957</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="7">
+        <v>-9.4583599412497203E-9</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J75" s="4">
+        <v>1</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L75" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M75" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N75" s="4">
+        <v>1</v>
+      </c>
+      <c r="O75" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P75" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q75" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R75" s="4">
+        <v>3</v>
+      </c>
+      <c r="S75" s="4">
+        <v>0.57209088006881903</v>
+      </c>
+      <c r="T75" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="9">
+        <v>1.6629947742052215E-3</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J76" s="4">
+        <v>2</v>
+      </c>
+      <c r="K76" s="4">
+        <v>-6.399135221166409</v>
+      </c>
+      <c r="L76" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M76" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N76" s="4">
+        <v>1</v>
+      </c>
+      <c r="O76" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P76" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q76" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R76" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S76" s="4">
+        <v>0.16169679924070957</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="9">
+        <v>8.31497387102593E-6</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J77" s="4">
+        <v>2</v>
+      </c>
+      <c r="K77" s="4">
+        <v>-11.697452587714467</v>
+      </c>
+      <c r="L77" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M77" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N77" s="4">
+        <v>1</v>
+      </c>
+      <c r="O77" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P77" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q77" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R77" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S77" s="4">
+        <v>0.16169679924070957</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B78" s="5">
+        <f>0.014966952967847/1000</f>
+        <v>1.4966952967847001E-5</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J78" s="4">
+        <v>2</v>
+      </c>
+      <c r="K78" s="4">
+        <v>-4.2019106438301899</v>
+      </c>
+      <c r="L78" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M78" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N78" s="4">
+        <v>1</v>
+      </c>
+      <c r="O78" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P78" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q78" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R78" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S78" s="4">
+        <v>0.16169679924070957</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" s="5">
+        <v>6.9444444444444448E-6</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J79" s="4">
+        <v>2</v>
+      </c>
+      <c r="K79" s="4">
+        <v>-11.877568578558138</v>
+      </c>
+      <c r="L79" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M79" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N79" s="4">
+        <v>1</v>
+      </c>
+      <c r="O79" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P79" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q79" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R79" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="S79" s="4">
+        <v>0.25816898211842121</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B80" s="9">
+        <v>8.31497387102593E-6</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M80" s="8"/>
+    </row>
+    <row r="81" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="5"/>
+    </row>
+    <row r="82" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M89" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N89" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O89" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P89" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q89" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R89" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T89" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U89" s="2"/>
+    </row>
+    <row r="90" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B90" s="5">
+        <v>1</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" s="7">
+        <v>6.2590774062544461E-7</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J91" s="4">
+        <v>2</v>
+      </c>
+      <c r="K91" s="4">
+        <v>-14.284062855900274</v>
+      </c>
+      <c r="L91" s="4">
+        <v>1</v>
+      </c>
+      <c r="M91" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N91" s="4">
+        <v>1</v>
+      </c>
+      <c r="O91" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P91" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q91" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R91" s="4">
+        <v>3</v>
+      </c>
+      <c r="S91" s="4">
+        <v>0.57157051623399524</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="9">
+        <v>2.0556127902646181E-3</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J92" s="4">
+        <v>2</v>
+      </c>
+      <c r="K92" s="4">
+        <v>-6.1871812807091953</v>
+      </c>
+      <c r="L92" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M92" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N92" s="4">
+        <v>1</v>
+      </c>
+      <c r="O92" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P92" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q92" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R92" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S92" s="4">
+        <v>0.16169679924070957</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="9">
+        <v>1.1511431625481964E-5</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J93" s="4">
+        <v>2</v>
+      </c>
+      <c r="K93" s="4">
+        <v>-11.37216996195022</v>
+      </c>
+      <c r="L93" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M93" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N93" s="4">
+        <v>1</v>
+      </c>
+      <c r="O93" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="P93" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q93" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R93" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S93" s="4">
+        <v>0.16169679924070957</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B94" s="5">
         <f>0.0185005151123816/1000</f>
         <v>1.8500515112381598E-5</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C94" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D94" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="F94" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H74" s="4" t="s">
+      <c r="H94" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I74" s="4" t="s">
+      <c r="I94" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J74" s="4">
-        <v>2</v>
-      </c>
-      <c r="K74" s="4">
+      <c r="J94" s="4">
+        <v>2</v>
+      </c>
+      <c r="K94" s="4">
         <v>-3.9899567033729753</v>
       </c>
-      <c r="L74" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M74" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N74" s="4">
-        <v>1</v>
-      </c>
-      <c r="O74" s="4">
+      <c r="L94" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M94" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N94" s="4">
+        <v>1</v>
+      </c>
+      <c r="O94" s="4">
         <v>1.01</v>
       </c>
-      <c r="P74" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q74" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R74" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S74" s="4">
+      <c r="P94" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q94" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R94" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S94" s="4">
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+    <row r="95" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B95" s="9">
         <v>1.1511431625481964E-5</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C95" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D95" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="F95" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H75" s="4" t="s">
+      <c r="H95" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I75" s="4" t="s">
+      <c r="I95" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="M75" s="8"/>
-    </row>
-    <row r="76" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="5"/>
-    </row>
-    <row r="77" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+      <c r="M95" s="8"/>
+    </row>
+    <row r="96" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="5"/>
+    </row>
+    <row r="97" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B78" s="5" t="s">
+    <row r="98" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+    <row r="99" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B99" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+    <row r="100" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="10" t="s">
+      <c r="B100" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+    <row r="101" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B101" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+    <row r="102" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B102" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
+    <row r="103" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B83" s="5"/>
-    </row>
-    <row r="84" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="B103" s="5"/>
+    </row>
+    <row r="104" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D104" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="E104" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="H104" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I84" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J84" s="2" t="s">
+      <c r="I104" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J104" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K84" s="2" t="s">
+      <c r="K104" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L84" s="2" t="s">
+      <c r="L104" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M84" s="2" t="s">
+      <c r="M104" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N84" s="2" t="s">
+      <c r="N104" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O84" s="2" t="s">
+      <c r="O104" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P84" s="2" t="s">
+      <c r="P104" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q84" s="2" t="s">
+      <c r="Q104" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R84" s="2" t="s">
+      <c r="R104" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S84" s="2" t="s">
+      <c r="S104" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T84" s="2" t="s">
+      <c r="T104" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U84" s="2"/>
-    </row>
-    <row r="85" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+      <c r="U104" s="2"/>
+    </row>
+    <row r="105" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B85" s="5">
-        <v>1</v>
-      </c>
-      <c r="C85" s="4" t="s">
+      <c r="B105" s="5">
+        <v>1</v>
+      </c>
+      <c r="C105" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E85" s="10" t="s">
+      <c r="E105" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F105" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G85" s="4" t="s">
+      <c r="G105" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
+    <row r="106" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B86" s="7">
+      <c r="B106" s="7">
         <v>1.0548435380476651E-9</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C106" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E86" s="10" t="s">
+      <c r="E106" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F86" s="4" t="s">
+      <c r="F106" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G86" s="4" t="s">
+      <c r="G106" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H86" s="4" t="s">
+      <c r="H106" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I86" s="4" t="s">
+      <c r="I106" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="J86" s="4">
-        <v>2</v>
-      </c>
-      <c r="K86" s="4">
+      <c r="J106" s="4">
+        <v>2</v>
+      </c>
+      <c r="K106" s="4">
         <v>-20.669873386184769</v>
       </c>
-      <c r="L86" s="4">
-        <v>1</v>
-      </c>
-      <c r="M86" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N86" s="4">
-        <v>1</v>
-      </c>
-      <c r="O86" s="4">
+      <c r="L106" s="4">
+        <v>1</v>
+      </c>
+      <c r="M106" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N106" s="4">
+        <v>1</v>
+      </c>
+      <c r="O106" s="4">
         <v>1.01</v>
       </c>
-      <c r="P86" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q86" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R86" s="4">
+      <c r="P106" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q106" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R106" s="4">
         <v>3</v>
       </c>
-      <c r="S86" s="4">
+      <c r="S106" s="4">
         <v>0.57157051623399524</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+    <row r="107" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B87" s="7">
+      <c r="B107" s="7">
         <v>1.0548435380476651E-9</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C107" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E87" s="10" t="s">
+      <c r="E107" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F87" s="4" t="s">
+      <c r="F107" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G87" s="4" t="s">
+      <c r="G107" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H87" s="4" t="s">
+      <c r="H107" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I87" s="4" t="s">
+      <c r="I107" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="J87" s="4">
-        <v>2</v>
-      </c>
-      <c r="K87" s="4">
+      <c r="J107" s="4">
+        <v>2</v>
+      </c>
+      <c r="K107" s="4">
         <v>-20.669873386184769</v>
       </c>
-      <c r="L87" s="4">
-        <v>1</v>
-      </c>
-      <c r="M87" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N87" s="4">
-        <v>1</v>
-      </c>
-      <c r="O87" s="4">
+      <c r="L107" s="4">
+        <v>1</v>
+      </c>
+      <c r="M107" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N107" s="4">
+        <v>1</v>
+      </c>
+      <c r="O107" s="4">
         <v>1.01</v>
       </c>
-      <c r="P87" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q87" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R87" s="4">
+      <c r="P107" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q107" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R107" s="4">
         <v>3</v>
       </c>
-      <c r="S87" s="4">
+      <c r="S107" s="4">
         <v>0.57157051623399524</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+    <row r="108" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B88" s="7">
+      <c r="B108" s="7">
         <v>1.9594773562773428E-6</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C108" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E88" s="10" t="s">
+      <c r="E108" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="F108" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G88" s="4" t="s">
+      <c r="G108" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H88" s="4" t="s">
+      <c r="H108" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J88" s="4">
-        <v>2</v>
-      </c>
-      <c r="K88" s="4">
+      <c r="J108" s="4">
+        <v>2</v>
+      </c>
+      <c r="K108" s="4">
         <v>-13.142832775241143</v>
       </c>
-      <c r="L88" s="4">
-        <v>1</v>
-      </c>
-      <c r="M88" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N88" s="4">
-        <v>1</v>
-      </c>
-      <c r="O88" s="4">
+      <c r="L108" s="4">
+        <v>1</v>
+      </c>
+      <c r="M108" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N108" s="4">
+        <v>1</v>
+      </c>
+      <c r="O108" s="4">
         <v>1.01</v>
       </c>
-      <c r="P88" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q88" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R88" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S88" s="4">
+      <c r="P108" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q108" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R108" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S108" s="4">
         <v>0.15984597228197622</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B89" s="9">
+    <row r="109" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" s="9">
         <v>2.061739642547709E-3</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C109" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E89" s="10" t="s">
+      <c r="E109" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="F109" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="G109" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H89" s="4" t="s">
+      <c r="H109" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="I109" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J89" s="4">
-        <v>2</v>
-      </c>
-      <c r="K89" s="4">
+      <c r="J109" s="4">
+        <v>2</v>
+      </c>
+      <c r="K109" s="4">
         <v>-6.1842051658852499</v>
       </c>
-      <c r="L89" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M89" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N89" s="4">
-        <v>1</v>
-      </c>
-      <c r="O89" s="4">
+      <c r="L109" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M109" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N109" s="4">
+        <v>1</v>
+      </c>
+      <c r="O109" s="4">
         <v>1.01</v>
       </c>
-      <c r="P89" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q89" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R89" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S89" s="4">
+      <c r="P109" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q109" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R109" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S109" s="4">
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B90" s="9">
+    <row r="110" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110" s="9">
         <v>1.1545741998267272E-5</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C110" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E90" s="10" t="s">
+      <c r="E110" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F90" s="4" t="s">
+      <c r="F110" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G90" s="4" t="s">
+      <c r="G110" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H90" s="4" t="s">
+      <c r="H110" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I90" s="4" t="s">
+      <c r="I110" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J90" s="4">
-        <v>2</v>
-      </c>
-      <c r="K90" s="4">
+      <c r="J110" s="4">
+        <v>2</v>
+      </c>
+      <c r="K110" s="4">
         <v>-11.369193847126274</v>
       </c>
-      <c r="L90" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M90" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N90" s="4">
-        <v>1</v>
-      </c>
-      <c r="O90" s="4">
+      <c r="L110" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M110" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N110" s="4">
+        <v>1</v>
+      </c>
+      <c r="O110" s="4">
         <v>1.01</v>
       </c>
-      <c r="P90" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q90" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R90" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S90" s="4">
+      <c r="P110" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q110" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R110" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S110" s="4">
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+    <row r="111" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B91" s="5">
+      <c r="B111" s="5">
         <f>0.0185556567829294/1000</f>
         <v>1.8555656782929398E-5</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C111" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D111" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F91" s="4" t="s">
+      <c r="F111" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H91" s="4" t="s">
+      <c r="H111" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I91" s="4" t="s">
+      <c r="I111" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J91" s="4">
-        <v>2</v>
-      </c>
-      <c r="K91" s="4">
+      <c r="J111" s="4">
+        <v>2</v>
+      </c>
+      <c r="K111" s="4">
         <v>-3.9869805885490299</v>
       </c>
-      <c r="L91" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="M91" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="N91" s="4">
-        <v>1</v>
-      </c>
-      <c r="O91" s="4">
+      <c r="L111" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="M111" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="N111" s="4">
+        <v>1</v>
+      </c>
+      <c r="O111" s="4">
         <v>1.01</v>
       </c>
-      <c r="P91" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="Q91" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="R91" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="S91" s="4">
+      <c r="P111" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="Q111" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="R111" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S111" s="4">
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+    <row r="112" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B92" s="9">
+      <c r="B112" s="9">
         <v>1.1545741998267272E-5</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C112" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D112" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F92" s="4" t="s">
+      <c r="F112" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H92" s="4" t="s">
+      <c r="H112" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I92" s="4" t="s">
+      <c r="I112" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="M92" s="8"/>
-    </row>
-    <row r="93" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="5"/>
+      <c r="M112" s="8"/>
+    </row>
+    <row r="113" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W93" xr:uid="{0E2FA153-E6EA-3E4B-BE1A-EC0443996927}"/>
+  <autoFilter ref="A1:W113" xr:uid="{0E2FA153-E6EA-3E4B-BE1A-EC0443996927}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix issue external scenario
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-heating.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-heating.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8828EB46-C4A9-704A-AE41-DDEE5691C2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98D162A-A2B2-7246-9839-D2307DA9EA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23000" xr2:uid="{CF516D2F-FFD4-214F-BF62-5C2F0868DC96}"/>
   </bookViews>
@@ -813,7 +813,7 @@
   <dimension ref="A1:W113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4356,5 +4356,6 @@
   </sheetData>
   <autoFilter ref="A1:W113" xr:uid="{0E2FA153-E6EA-3E4B-BE1A-EC0443996927}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add final energy mapping file.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-heating.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-heating.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65336C7-DDA1-C244-9BF5-71DE7F09D2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2ADA8E-AB59-4548-B1A6-B93BFCC42BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31900" yWindow="-760" windowWidth="30240" windowHeight="18880" xr2:uid="{CF516D2F-FFD4-214F-BF62-5C2F0868DC96}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CF516D2F-FFD4-214F-BF62-5C2F0868DC96}"/>
   </bookViews>
   <sheets>
     <sheet name="hydrogen boiler" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'hydrogen boiler'!$A$1:$W$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'hydrogen boiler'!$A$1:$W$292</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -993,10 +993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2FA153-E6EA-3E4B-BE1A-EC0443996927}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="C269" sqref="C269"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G293" sqref="G293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1016,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1063,7 +1066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1090,7 +1093,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1156,7 @@
       </c>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1730,7 +1733,8 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -1738,7 +1742,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>1</v>
       </c>
@@ -1746,7 +1750,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
@@ -1754,7 +1758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>4</v>
       </c>
@@ -1762,7 +1766,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
@@ -1770,7 +1774,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -1778,13 +1782,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -1847,7 +1851,7 @@
       </c>
       <c r="U31" s="2"/>
     </row>
-    <row r="32" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>88</v>
       </c>
@@ -1867,7 +1871,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>59</v>
       </c>
@@ -1923,7 +1927,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="34" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>63</v>
       </c>
@@ -1979,7 +1983,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>109</v>
       </c>
@@ -2035,7 +2039,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -2091,7 +2095,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>113</v>
       </c>
@@ -2147,7 +2151,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>83</v>
       </c>
@@ -2201,7 +2205,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="39" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>85</v>
       </c>
@@ -2254,7 +2258,7 @@
         <v>0.25816898211842121</v>
       </c>
     </row>
-    <row r="40" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
@@ -2278,10 +2282,10 @@
       </c>
       <c r="M40" s="8"/>
     </row>
-    <row r="41" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" s="5"/>
     </row>
-    <row r="42" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2293,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>1</v>
       </c>
@@ -2297,7 +2301,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>2</v>
       </c>
@@ -2305,7 +2309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>4</v>
       </c>
@@ -2313,7 +2317,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>5</v>
       </c>
@@ -2321,7 +2325,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -2329,13 +2333,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="5"/>
     </row>
-    <row r="49" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
@@ -2398,7 +2402,7 @@
       </c>
       <c r="U49" s="2"/>
     </row>
-    <row r="50" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>102</v>
       </c>
@@ -2418,7 +2422,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>92</v>
       </c>
@@ -2474,7 +2478,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="52" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>94</v>
       </c>
@@ -2530,7 +2534,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>96</v>
       </c>
@@ -2586,7 +2590,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="54" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>73</v>
       </c>
@@ -2639,7 +2643,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>76</v>
       </c>
@@ -2695,7 +2699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -2751,7 +2755,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>113</v>
       </c>
@@ -2807,7 +2811,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="58" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>83</v>
       </c>
@@ -2861,7 +2865,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>85</v>
       </c>
@@ -2914,7 +2918,7 @@
         <v>0.25816898211842121</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>53</v>
       </c>
@@ -2938,10 +2942,10 @@
       </c>
       <c r="M60" s="8"/>
     </row>
-    <row r="61" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" s="5"/>
     </row>
-    <row r="62" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>0</v>
       </c>
@@ -2949,7 +2953,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>1</v>
       </c>
@@ -2957,7 +2961,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>2</v>
       </c>
@@ -2965,7 +2969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>4</v>
       </c>
@@ -2973,7 +2977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>5</v>
       </c>
@@ -2981,7 +2985,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>7</v>
       </c>
@@ -2989,13 +2993,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B68" s="5"/>
     </row>
-    <row r="69" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>12</v>
       </c>
@@ -3058,7 +3062,7 @@
       </c>
       <c r="U69" s="2"/>
     </row>
-    <row r="70" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>104</v>
       </c>
@@ -3078,7 +3082,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>98</v>
       </c>
@@ -3134,7 +3138,7 @@
         <v>0.57157051623399524</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>113</v>
       </c>
@@ -3190,7 +3194,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>113</v>
       </c>
@@ -3246,7 +3250,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="74" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>83</v>
       </c>
@@ -3300,7 +3304,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>53</v>
       </c>
@@ -3324,10 +3328,10 @@
       </c>
       <c r="M75" s="8"/>
     </row>
-    <row r="76" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" s="5"/>
     </row>
-    <row r="77" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>0</v>
       </c>
@@ -3335,7 +3339,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>1</v>
       </c>
@@ -3343,7 +3347,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>2</v>
       </c>
@@ -3351,7 +3355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>4</v>
       </c>
@@ -3359,7 +3363,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>5</v>
       </c>
@@ -3367,7 +3371,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>7</v>
       </c>
@@ -3375,13 +3379,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B83" s="5"/>
     </row>
-    <row r="84" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>12</v>
       </c>
@@ -3444,7 +3448,7 @@
       </c>
       <c r="U84" s="2"/>
     </row>
-    <row r="85" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>106</v>
       </c>
@@ -3464,7 +3468,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>100</v>
       </c>
@@ -3520,7 +3524,7 @@
         <v>0.57157051623399524</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>70</v>
       </c>
@@ -3576,7 +3580,7 @@
         <v>0.57157051623399524</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>78</v>
       </c>
@@ -3629,7 +3633,7 @@
         <v>0.15984597228197622</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>113</v>
       </c>
@@ -3685,7 +3689,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>113</v>
       </c>
@@ -3741,7 +3745,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>83</v>
       </c>
@@ -3795,7 +3799,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>53</v>
       </c>
@@ -3819,10 +3823,10 @@
       </c>
       <c r="M92" s="8"/>
     </row>
-    <row r="93" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B93" s="5"/>
     </row>
-    <row r="94" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>0</v>
       </c>
@@ -3830,7 +3834,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>1</v>
       </c>
@@ -3838,7 +3842,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>2</v>
       </c>
@@ -3846,7 +3850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>4</v>
       </c>
@@ -3854,7 +3858,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>5</v>
       </c>
@@ -3862,7 +3866,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="99" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>7</v>
       </c>
@@ -3870,16 +3874,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B100" s="5"/>
     </row>
-    <row r="101" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B101" s="5"/>
     </row>
-    <row r="102" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>12</v>
       </c>
@@ -3950,7 +3954,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="103" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>127</v>
       </c>
@@ -3976,7 +3980,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="104" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>92</v>
       </c>
@@ -4038,7 +4042,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="105" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>94</v>
       </c>
@@ -4100,7 +4104,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="106" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>96</v>
       </c>
@@ -4162,7 +4166,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="107" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>73</v>
       </c>
@@ -4218,7 +4222,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="108" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>76</v>
       </c>
@@ -4277,7 +4281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>113</v>
       </c>
@@ -4339,7 +4343,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="110" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>113</v>
       </c>
@@ -4401,7 +4405,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="111" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>83</v>
       </c>
@@ -4458,7 +4462,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="112" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>85</v>
       </c>
@@ -4514,7 +4518,7 @@
         <v>0.25816898211842121</v>
       </c>
     </row>
-    <row r="113" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>53</v>
       </c>
@@ -4541,10 +4545,10 @@
       </c>
       <c r="O113" s="8"/>
     </row>
-    <row r="114" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B114" s="5"/>
     </row>
-    <row r="115" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>0</v>
       </c>
@@ -4552,7 +4556,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="116" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>1</v>
       </c>
@@ -4560,7 +4564,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>2</v>
       </c>
@@ -4568,7 +4572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>4</v>
       </c>
@@ -4576,7 +4580,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="119" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>5</v>
       </c>
@@ -4584,7 +4588,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="120" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>7</v>
       </c>
@@ -4592,16 +4596,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" s="5"/>
     </row>
-    <row r="122" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B122" s="5"/>
     </row>
-    <row r="123" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>12</v>
       </c>
@@ -4672,7 +4676,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="124" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>130</v>
       </c>
@@ -4698,7 +4702,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>98</v>
       </c>
@@ -4760,7 +4764,7 @@
         <v>0.57157051623399524</v>
       </c>
     </row>
-    <row r="126" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>113</v>
       </c>
@@ -4822,7 +4826,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="127" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>113</v>
       </c>
@@ -4884,7 +4888,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="128" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>83</v>
       </c>
@@ -4941,7 +4945,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="129" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>53</v>
       </c>
@@ -4968,10 +4972,10 @@
       </c>
       <c r="O129" s="8"/>
     </row>
-    <row r="130" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B130" s="5"/>
     </row>
-    <row r="131" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>0</v>
       </c>
@@ -4979,7 +4983,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="132" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>1</v>
       </c>
@@ -4987,7 +4991,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="133" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>2</v>
       </c>
@@ -4995,7 +4999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>4</v>
       </c>
@@ -5003,7 +5007,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="135" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>5</v>
       </c>
@@ -5011,7 +5015,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="136" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>7</v>
       </c>
@@ -5019,16 +5023,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="137" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B137" s="5"/>
     </row>
-    <row r="138" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B138" s="5"/>
     </row>
-    <row r="139" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>12</v>
       </c>
@@ -5099,7 +5103,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="140" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>132</v>
       </c>
@@ -5125,7 +5129,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="141" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>100</v>
       </c>
@@ -5187,7 +5191,7 @@
         <v>0.57157051623399524</v>
       </c>
     </row>
-    <row r="142" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>70</v>
       </c>
@@ -5246,7 +5250,7 @@
         <v>0.57157051623399524</v>
       </c>
     </row>
-    <row r="143" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>78</v>
       </c>
@@ -5302,7 +5306,7 @@
         <v>0.15984597228197622</v>
       </c>
     </row>
-    <row r="144" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>113</v>
       </c>
@@ -5364,7 +5368,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="145" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>113</v>
       </c>
@@ -5426,7 +5430,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="146" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>83</v>
       </c>
@@ -5483,7 +5487,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="147" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>53</v>
       </c>
@@ -5510,10 +5514,10 @@
       </c>
       <c r="O147" s="8"/>
     </row>
-    <row r="148" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:23" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B148" s="5"/>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -5521,7 +5525,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>1</v>
       </c>
@@ -5529,7 +5533,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>2</v>
       </c>
@@ -5537,7 +5541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>4</v>
       </c>
@@ -5545,7 +5549,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>5</v>
       </c>
@@ -5553,12 +5557,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="154" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:23" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:23" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>12</v>
       </c>
@@ -5629,7 +5633,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>134</v>
       </c>
@@ -5655,7 +5659,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>59</v>
       </c>
@@ -5714,7 +5718,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>63</v>
       </c>
@@ -5773,7 +5777,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>109</v>
       </c>
@@ -5835,7 +5839,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>167</v>
       </c>
@@ -5897,7 +5901,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>141</v>
       </c>
@@ -5953,7 +5957,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>144</v>
       </c>
@@ -6009,7 +6013,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>145</v>
       </c>
@@ -6065,7 +6069,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>146</v>
       </c>
@@ -6121,7 +6125,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>147</v>
       </c>
@@ -6153,7 +6157,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>148</v>
       </c>
@@ -6209,7 +6213,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>149</v>
       </c>
@@ -6265,7 +6269,7 @@
         <v>0.93208283513358414</v>
       </c>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>150</v>
       </c>
@@ -6321,7 +6325,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>151</v>
       </c>
@@ -6377,7 +6381,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>152</v>
       </c>
@@ -6433,7 +6437,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>153</v>
       </c>
@@ -6489,7 +6493,7 @@
         <v>0.93208283513358414</v>
       </c>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>154</v>
       </c>
@@ -6545,7 +6549,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>155</v>
       </c>
@@ -6577,7 +6581,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>85</v>
       </c>
@@ -6633,7 +6637,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>156</v>
       </c>
@@ -6689,7 +6693,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>157</v>
       </c>
@@ -6745,7 +6749,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>158</v>
       </c>
@@ -6801,7 +6805,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>159</v>
       </c>
@@ -6857,7 +6861,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>160</v>
       </c>
@@ -6913,7 +6917,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>161</v>
       </c>
@@ -6969,7 +6973,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>162</v>
       </c>
@@ -7025,7 +7029,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>164</v>
       </c>
@@ -7081,7 +7085,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>165</v>
       </c>
@@ -7137,7 +7141,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>166</v>
       </c>
@@ -7193,7 +7197,8 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:23" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="186" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>0</v>
       </c>
@@ -7201,7 +7206,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>1</v>
       </c>
@@ -7209,7 +7214,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>2</v>
       </c>
@@ -7217,7 +7222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>4</v>
       </c>
@@ -7225,7 +7230,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>5</v>
       </c>
@@ -7233,12 +7238,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="191" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:23" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:23" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>12</v>
       </c>
@@ -7309,7 +7314,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="str">
         <f>B186</f>
         <v>heat, residential, by combustion of coal-based natural gas using boiler, distributed by pipeline</v>
@@ -7336,7 +7341,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>59</v>
       </c>
@@ -7395,7 +7400,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>63</v>
       </c>
@@ -7454,7 +7459,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>109</v>
       </c>
@@ -7516,7 +7521,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>170</v>
       </c>
@@ -7578,7 +7583,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>141</v>
       </c>
@@ -7634,7 +7639,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>144</v>
       </c>
@@ -7690,7 +7695,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>145</v>
       </c>
@@ -7746,7 +7751,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>146</v>
       </c>
@@ -7802,7 +7807,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>147</v>
       </c>
@@ -7834,7 +7839,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>172</v>
       </c>
@@ -7890,7 +7895,7 @@
         <v>0.93208283513358414</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>150</v>
       </c>
@@ -7946,7 +7951,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>151</v>
       </c>
@@ -8002,7 +8007,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>152</v>
       </c>
@@ -8058,7 +8063,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>153</v>
       </c>
@@ -8114,7 +8119,7 @@
         <v>0.93208283513358414</v>
       </c>
     </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>155</v>
       </c>
@@ -8170,7 +8175,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="209" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>155</v>
       </c>
@@ -8202,7 +8207,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="210" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>85</v>
       </c>
@@ -8258,7 +8263,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="211" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>156</v>
       </c>
@@ -8314,7 +8319,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="212" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>157</v>
       </c>
@@ -8370,7 +8375,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="213" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>158</v>
       </c>
@@ -8426,7 +8431,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>159</v>
       </c>
@@ -8482,7 +8487,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="215" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>160</v>
       </c>
@@ -8538,7 +8543,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="216" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>161</v>
       </c>
@@ -8594,7 +8599,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="217" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>162</v>
       </c>
@@ -8650,7 +8655,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="218" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>164</v>
       </c>
@@ -8706,7 +8711,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="219" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>165</v>
       </c>
@@ -8762,7 +8767,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="220" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>166</v>
       </c>
@@ -8818,7 +8823,8 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="222" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:21" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="222" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>0</v>
       </c>
@@ -8826,7 +8832,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="223" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>1</v>
       </c>
@@ -8834,7 +8840,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="224" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>2</v>
       </c>
@@ -8842,7 +8848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>4</v>
       </c>
@@ -8850,7 +8856,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>5</v>
       </c>
@@ -8858,12 +8864,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="227" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:23" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:23" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>12</v>
       </c>
@@ -8961,7 +8967,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>59</v>
       </c>
@@ -9020,7 +9026,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>63</v>
       </c>
@@ -9079,7 +9085,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>109</v>
       </c>
@@ -9158,7 +9164,7 @@
         <v>29</v>
       </c>
       <c r="G233" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="H233" t="s">
         <v>175</v>
@@ -9203,7 +9209,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>141</v>
       </c>
@@ -9259,7 +9265,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>144</v>
       </c>
@@ -9315,7 +9321,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>145</v>
       </c>
@@ -9371,7 +9377,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>146</v>
       </c>
@@ -9427,7 +9433,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>148</v>
       </c>
@@ -9483,7 +9489,7 @@
         <v>0.47095746419981693</v>
       </c>
     </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>149</v>
       </c>
@@ -9539,7 +9545,7 @@
         <v>0.93208283513358414</v>
       </c>
     </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>150</v>
       </c>
@@ -9595,7 +9601,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="241" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>151</v>
       </c>
@@ -9651,7 +9657,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="242" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>152</v>
       </c>
@@ -9707,7 +9713,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="243" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>153</v>
       </c>
@@ -9763,7 +9769,7 @@
         <v>0.93208283513358414</v>
       </c>
     </row>
-    <row r="244" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>154</v>
       </c>
@@ -9819,7 +9825,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="245" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>155</v>
       </c>
@@ -9851,7 +9857,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="246" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>85</v>
       </c>
@@ -9907,7 +9913,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="247" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>156</v>
       </c>
@@ -9963,7 +9969,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="248" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>157</v>
       </c>
@@ -10019,7 +10025,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="249" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>158</v>
       </c>
@@ -10075,7 +10081,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>159</v>
       </c>
@@ -10131,7 +10137,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="251" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>160</v>
       </c>
@@ -10187,7 +10193,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="252" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>161</v>
       </c>
@@ -10243,7 +10249,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="253" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>162</v>
       </c>
@@ -10299,7 +10305,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="254" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>164</v>
       </c>
@@ -10355,7 +10361,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="255" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>165</v>
       </c>
@@ -10411,7 +10417,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="256" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>166</v>
       </c>
@@ -10467,7 +10473,8 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="258" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:23" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="258" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>0</v>
       </c>
@@ -10475,7 +10482,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="259" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>1</v>
       </c>
@@ -10483,7 +10490,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="260" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>2</v>
       </c>
@@ -10491,7 +10498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>4</v>
       </c>
@@ -10499,7 +10506,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="262" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>5</v>
       </c>
@@ -10507,12 +10514,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="263" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:23" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="264" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:23" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>12</v>
       </c>
@@ -10583,7 +10590,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="265" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="str">
         <f>B258</f>
         <v>heat, residential, by combustion of liquefied petroleum gas using boiler, distributed by pipeline</v>
@@ -10610,7 +10617,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="266" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>59</v>
       </c>
@@ -10669,7 +10676,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="267" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>63</v>
       </c>
@@ -10728,7 +10735,7 @@
         <v>0.57209088006881903</v>
       </c>
     </row>
-    <row r="268" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>109</v>
       </c>
@@ -10790,7 +10797,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="269" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>180</v>
       </c>
@@ -10852,7 +10859,7 @@
         <v>0.16169679924070957</v>
       </c>
     </row>
-    <row r="270" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>141</v>
       </c>
@@ -10908,7 +10915,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="271" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>144</v>
       </c>
@@ -10964,7 +10971,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="272" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>145</v>
       </c>
@@ -11020,7 +11027,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="273" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>146</v>
       </c>
@@ -11076,7 +11083,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="274" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>147</v>
       </c>
@@ -11108,7 +11115,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="275" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>172</v>
       </c>
@@ -11164,7 +11171,7 @@
         <v>0.93208283513358414</v>
       </c>
     </row>
-    <row r="276" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>150</v>
       </c>
@@ -11220,7 +11227,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="277" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>151</v>
       </c>
@@ -11276,7 +11283,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="278" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>152</v>
       </c>
@@ -11332,7 +11339,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="279" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>153</v>
       </c>
@@ -11388,7 +11395,7 @@
         <v>0.93208283513358414</v>
       </c>
     </row>
-    <row r="280" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>155</v>
       </c>
@@ -11444,7 +11451,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="281" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>155</v>
       </c>
@@ -11476,7 +11483,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="282" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>85</v>
       </c>
@@ -11532,7 +11539,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="283" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>156</v>
       </c>
@@ -11588,7 +11595,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="284" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>157</v>
       </c>
@@ -11644,7 +11651,7 @@
         <v>0.72314801614797197</v>
       </c>
     </row>
-    <row r="285" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>158</v>
       </c>
@@ -11700,7 +11707,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="286" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>159</v>
       </c>
@@ -11756,7 +11763,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="287" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>160</v>
       </c>
@@ -11812,7 +11819,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>161</v>
       </c>
@@ -11868,7 +11875,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="289" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>162</v>
       </c>
@@ -11924,7 +11931,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="290" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>164</v>
       </c>
@@ -11980,7 +11987,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="291" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>165</v>
       </c>
@@ -12036,7 +12043,7 @@
         <v>0.51215847306170115</v>
       </c>
     </row>
-    <row r="292" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>166</v>
       </c>
@@ -12093,7 +12100,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W93" xr:uid="{0E2FA153-E6EA-3E4B-BE1A-EC0443996927}"/>
+  <autoFilter ref="A1:W292" xr:uid="{0E2FA153-E6EA-3E4B-BE1A-EC0443996927}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="biomethane, gaseous, 5 bar, from sewage sludge fermentation, at fuelling station"/>
+        <filter val="heat, residential, by combustion of biomethane using boiler, distributed by pipeline"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>